<commit_message>
clinical roster v0.1.0 + intern v5.4
Intern run time > 20 hours - not complete
clinical roster > 18,000 lines output - less feasible to copy to excel
</commit_message>
<xml_diff>
--- a/Clinical Roster/Clinical Roster/Clinical Roster Index.xlsx
+++ b/Clinical Roster/Clinical Roster/Clinical Roster Index.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\SLE352 CSP\Repo\Rostering\Clinical Roster\Clinical Roster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B10A94CD-43AD-474B-B18C-1C8C20C868EA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2912CF57-162B-4B12-9F83-0C883D94D33C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F2F070BB-8F06-4968-B2A9-E073D47483C9}"/>
+    <workbookView xWindow="-18380" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{F2F070BB-8F06-4968-B2A9-E073D47483C9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="p" sheetId="1" r:id="rId1"/>
+    <sheet name="d" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
   <si>
     <t>Clinical Roster Index</t>
   </si>
@@ -157,13 +158,166 @@
   </si>
   <si>
     <t>Blank</t>
+  </si>
+  <si>
+    <t>EFT</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>M,F</t>
+  </si>
+  <si>
+    <t>Tu,W,Th</t>
+  </si>
+  <si>
+    <t>Tu,F</t>
+  </si>
+  <si>
+    <t>M,W,Th</t>
+  </si>
+  <si>
+    <t>Silvana</t>
+  </si>
+  <si>
+    <t>W,Th</t>
+  </si>
+  <si>
+    <t>Th,F</t>
+  </si>
+  <si>
+    <t>Tu,Th</t>
+  </si>
+  <si>
+    <t>M,Th,F</t>
+  </si>
+  <si>
+    <t>Tu,W</t>
+  </si>
+  <si>
+    <t>W,Th,F</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>RHEUM / ENDO / DERM (RhEnDe)</t>
+  </si>
+  <si>
+    <t>HAEM WHITE</t>
+  </si>
+  <si>
+    <t>HAEM RED</t>
+  </si>
+  <si>
+    <t>NEURO/STROKE</t>
+  </si>
+  <si>
+    <t>NEUROSURG</t>
+  </si>
+  <si>
+    <t>ID / IMMUNO / PALL CARE (8.30-5)</t>
+  </si>
+  <si>
+    <t>TB / HIV SERVICES</t>
+  </si>
+  <si>
+    <t>RESP/CF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(8am-4.30pm)  42 ECHO </t>
+  </si>
+  <si>
+    <t>(8am-4.30pm) 42 DELTA (+outliers)</t>
+  </si>
+  <si>
+    <t>(8am-4.30pm) 41 BRAVO</t>
+  </si>
+  <si>
+    <t>(8am-4.30pm) 41 ALPHA (+outliers)</t>
+  </si>
+  <si>
+    <t>(8am-4.30pm) ADMISSIONS</t>
+  </si>
+  <si>
+    <t>(8am-4.30pm) ADMISSIONS/ DISCHARGE SUPPORT</t>
+  </si>
+  <si>
+    <t>(11.30am-8pm) LATE</t>
+  </si>
+  <si>
+    <t>(11.30am - 8pm) PPMC late</t>
+  </si>
+  <si>
+    <t>NEPHROLOGY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RENAL TRANSPLANT/ENDO SURG </t>
+  </si>
+  <si>
+    <t>(8am-4.30pm) GASTRO 34 / CLINICS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GASTRO&amp;SURG helper/MENTAL HEALTH (MBU,STEPPING STONES)</t>
+  </si>
+  <si>
+    <t>MENTAL HEALTH (ADPS)</t>
+  </si>
+  <si>
+    <t>(8am-4.30pm) AAC</t>
+  </si>
+  <si>
+    <t>(8am-4.30pm) UPPER GI / GEN SURG (including outliers) 33</t>
+  </si>
+  <si>
+    <t>VASCULAR/SPECIALTY SURGERY (UROL/ GYNAE/ DENT/ ENT/ Plastics/ OPTHAL/MAX FAX)</t>
+  </si>
+  <si>
+    <t>ICU</t>
+  </si>
+  <si>
+    <t>ICU / CARDIOLOGY</t>
+  </si>
+  <si>
+    <t>(8am-4.30pm) CARDIOLOGY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(8am-4.30pm) CTS </t>
+  </si>
+  <si>
+    <t>(8am-4.30pm) EMERGENCY</t>
+  </si>
+  <si>
+    <t>EMERGENCY / DISPENSARY</t>
+  </si>
+  <si>
+    <t>ANNUAL LEAVE</t>
+  </si>
+  <si>
+    <t>ADO ROSTERED</t>
+  </si>
+  <si>
+    <t>LATE SHIFT</t>
+  </si>
+  <si>
+    <t>TIME IN LIEU</t>
+  </si>
+  <si>
+    <t>LONG SERVICE LEAVE</t>
+  </si>
+  <si>
+    <t>PROFESSIONAL DEVELOPMENT</t>
+  </si>
+  <si>
+    <t>ROSTERED SICK/CARERS LEAVE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,8 +333,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,30 +357,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE05956"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -220,26 +394,237 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{3DFD0E7C-915F-46CC-A52D-81A3C03F989E}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -554,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E202B4A4-0B67-4757-82E8-1CBD3BF89141}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,115 +951,175 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
+      <c r="C3">
+        <v>0.4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="7">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
+      <c r="C4">
+        <v>0.6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="7">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="C5">
+        <v>0.4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="7">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="C6">
+        <v>0.6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="7">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="7">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="7">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="7">
         <v>9</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="7">
         <v>10</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="C12">
+        <v>0.4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="7">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>0.4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="B14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>14</v>
+      <c r="C14">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -682,7 +1127,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -690,222 +1138,326 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>22</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>23</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
-        <v>23</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>0.4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>24</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="C26">
+        <v>0.6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>25</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="C27">
+        <v>0.4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>26</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>27</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>28</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>29</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>30</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>31</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>32</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>33</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="6">
-        <v>33</v>
-      </c>
-      <c r="B35" s="6" t="s">
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="14">
+        <v>34</v>
+      </c>
+      <c r="B36" s="14" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="6">
-        <v>34</v>
-      </c>
-      <c r="B36" s="6" t="s">
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="14">
+        <v>35</v>
+      </c>
+      <c r="B37" s="14" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="6">
-        <v>35</v>
-      </c>
-      <c r="B37" s="6" t="s">
+      <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="14">
+        <v>36</v>
+      </c>
+      <c r="B38" s="14" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="6">
-        <v>36</v>
-      </c>
-      <c r="B38" s="6" t="s">
+      <c r="C38">
+        <v>0.6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="14">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="6">
+      <c r="B39" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="14">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="6">
+      <c r="B40" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="C40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="14">
+        <v>39</v>
+      </c>
+      <c r="B41" s="14" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="6">
-        <v>39</v>
-      </c>
-      <c r="B41" s="6" t="s">
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="14">
+        <v>40</v>
+      </c>
+      <c r="B42" s="14" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="6">
-        <v>40</v>
-      </c>
-      <c r="B42" s="6" t="s">
+      <c r="C42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="14">
+        <v>41</v>
+      </c>
+      <c r="B43" s="14" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>41</v>
-      </c>
-      <c r="B43" s="7" t="s">
+      <c r="C43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>42</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>43</v>
       </c>
     </row>
@@ -916,4 +1468,389 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7A5C92-D8DA-4BB8-AAAB-8EF9C4F97147}">
+  <dimension ref="A1:B38"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="81.7109375" style="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B8">
+    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="COVER">
+      <formula>NOT(ISERROR(SEARCH("COVER",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B9">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="blank">
+      <formula>NOT(ISERROR(SEARCH("blank",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="qq">
+      <formula>NOT(ISERROR(SEARCH("qq",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Public Holiday">
+      <formula>NOT(ISERROR(SEARCH("Public Holiday",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10:B17">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="COVER">
+      <formula>NOT(ISERROR(SEARCH("COVER",B10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="blank">
+      <formula>NOT(ISERROR(SEARCH("blank",B10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18:B25">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="COVER">
+      <formula>NOT(ISERROR(SEARCH("COVER",B18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="blank">
+      <formula>NOT(ISERROR(SEARCH("blank",B18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26:B31">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="COVER">
+      <formula>NOT(ISERROR(SEARCH("COVER",B26)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="blank">
+      <formula>NOT(ISERROR(SEARCH("blank",B26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34:B38">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="qq">
+      <formula>NOT(ISERROR(SEARCH("qq",B34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Public Holiday">
+      <formula>NOT(ISERROR(SEARCH("Public Holiday",B34)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="blank">
+      <formula>NOT(ISERROR(SEARCH("blank",B34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32:B33">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="qq">
+      <formula>NOT(ISERROR(SEARCH("qq",B32)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Public Holiday">
+      <formula>NOT(ISERROR(SEARCH("Public Holiday",B32)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="blank">
+      <formula>NOT(ISERROR(SEARCH("blank",B32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
v5.5 - still problematic
</commit_message>
<xml_diff>
--- a/Clinical Roster/Clinical Roster/Clinical Roster Index.xlsx
+++ b/Clinical Roster/Clinical Roster/Clinical Roster Index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\SLE352 CSP\Repo\Rostering\Clinical Roster\Clinical Roster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2912CF57-162B-4B12-9F83-0C883D94D33C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57DE1277-1C94-4F58-96A3-F0D8C23349E0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18380" yWindow="-110" windowWidth="18490" windowHeight="11020" xr2:uid="{F2F070BB-8F06-4968-B2A9-E073D47483C9}"/>
+    <workbookView xWindow="-9320" yWindow="180" windowWidth="8870" windowHeight="10350" activeTab="1" xr2:uid="{913E61F9-9BD4-4F8C-9B5A-94B900C198BB}"/>
   </bookViews>
   <sheets>
     <sheet name="p" sheetId="1" r:id="rId1"/>
@@ -220,9 +220,6 @@
     <t>ID / IMMUNO / PALL CARE (8.30-5)</t>
   </si>
   <si>
-    <t>TB / HIV SERVICES</t>
-  </si>
-  <si>
     <t>RESP/CF</t>
   </si>
   <si>
@@ -265,9 +262,6 @@
     <t>MENTAL HEALTH (ADPS)</t>
   </si>
   <si>
-    <t>(8am-4.30pm) AAC</t>
-  </si>
-  <si>
     <t>(8am-4.30pm) UPPER GI / GEN SURG (including outliers) 33</t>
   </si>
   <si>
@@ -311,6 +305,12 @@
   </si>
   <si>
     <t>ROSTERED SICK/CARERS LEAVE</t>
+  </si>
+  <si>
+    <t>TB / HIV SERVICES (W + F)</t>
+  </si>
+  <si>
+    <t>(8am-4.30pm) AAC (M, Tu, W, Th)</t>
   </si>
 </sst>
 </file>
@@ -431,9 +431,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -457,6 +454,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -941,8 +941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E202B4A4-0B67-4757-82E8-1CBD3BF89141}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,12 +951,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -973,10 +973,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
-        <v>1</v>
-      </c>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C3">
@@ -987,10 +987,10 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C4">
@@ -1001,10 +1001,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C5">
@@ -1015,10 +1015,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>4</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C6">
@@ -1029,10 +1029,10 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C7">
@@ -1040,10 +1040,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <v>6</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C8">
@@ -1051,10 +1051,10 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>7</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C9">
@@ -1062,10 +1062,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>8</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C10">
@@ -1073,10 +1073,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>9</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C11">
@@ -1084,10 +1084,10 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="6">
         <v>10</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C12">
@@ -1098,10 +1098,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+      <c r="A13" s="6">
         <v>11</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>50</v>
       </c>
       <c r="C13">
@@ -1112,10 +1112,10 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
+      <c r="A14" s="6">
         <v>12</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C14">
@@ -1123,10 +1123,10 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>13</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C15">
@@ -1134,10 +1134,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>14</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C16">
@@ -1145,10 +1145,10 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>15</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C17">
@@ -1156,10 +1156,10 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>16</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C18">
@@ -1167,10 +1167,10 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>17</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C19">
@@ -1178,10 +1178,10 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>18</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C20">
@@ -1189,10 +1189,10 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>19</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C21">
@@ -1200,10 +1200,10 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>20</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C22">
@@ -1211,10 +1211,10 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>21</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C23">
@@ -1222,10 +1222,10 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>22</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C24">
@@ -1233,10 +1233,10 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>23</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C25">
@@ -1247,10 +1247,10 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="A26" s="4">
         <v>24</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C26">
@@ -1261,10 +1261,10 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+      <c r="A27" s="4">
         <v>25</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C27">
@@ -1275,10 +1275,10 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+      <c r="A28" s="4">
         <v>26</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C28">
@@ -1286,10 +1286,10 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
+      <c r="A29" s="4">
         <v>27</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C29">
@@ -1297,10 +1297,10 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+      <c r="A30" s="4">
         <v>28</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C30">
@@ -1308,10 +1308,10 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
+      <c r="A31" s="4">
         <v>29</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C31">
@@ -1319,10 +1319,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
+      <c r="A32" s="4">
         <v>30</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C32">
@@ -1330,10 +1330,10 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
+      <c r="A33" s="4">
         <v>31</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C33">
@@ -1341,10 +1341,10 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
+      <c r="A34" s="4">
         <v>32</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C34">
@@ -1352,10 +1352,10 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
+      <c r="A35" s="4">
         <v>33</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C35">
@@ -1363,10 +1363,10 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="14">
+      <c r="A36" s="13">
         <v>34</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="13" t="s">
         <v>35</v>
       </c>
       <c r="C36">
@@ -1374,10 +1374,10 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="14">
+      <c r="A37" s="13">
         <v>35</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="13" t="s">
         <v>36</v>
       </c>
       <c r="C37">
@@ -1385,10 +1385,10 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="14">
+      <c r="A38" s="13">
         <v>36</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="13" t="s">
         <v>39</v>
       </c>
       <c r="C38">
@@ -1399,10 +1399,10 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="14">
+      <c r="A39" s="13">
         <v>37</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="13" t="s">
         <v>37</v>
       </c>
       <c r="C39">
@@ -1410,10 +1410,10 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="14">
+      <c r="A40" s="13">
         <v>38</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="13" t="s">
         <v>38</v>
       </c>
       <c r="C40">
@@ -1421,10 +1421,10 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="14">
+      <c r="A41" s="13">
         <v>39</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="13" t="s">
         <v>40</v>
       </c>
       <c r="C41">
@@ -1432,10 +1432,10 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="14">
+      <c r="A42" s="13">
         <v>40</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="13" t="s">
         <v>41</v>
       </c>
       <c r="C42">
@@ -1443,10 +1443,10 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="14">
+      <c r="A43" s="13">
         <v>41</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="13" t="s">
         <v>42</v>
       </c>
       <c r="C43">
@@ -1474,20 +1474,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E7A5C92-D8DA-4BB8-AAAB-8EF9C4F97147}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="81.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="81.7109375" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1495,7 +1493,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1503,7 +1501,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1511,7 +1509,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1519,7 +1517,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1527,7 +1525,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1535,7 +1533,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1543,248 +1541,248 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>64</v>
+      <c r="B8" s="5" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>65</v>
+      <c r="B9" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>66</v>
+      <c r="B10" s="8" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>67</v>
+      <c r="B11" s="8" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>68</v>
+      <c r="B12" s="8" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>69</v>
+      <c r="B13" s="8" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>70</v>
+      <c r="B14" s="8" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>71</v>
+      <c r="B15" s="8" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>72</v>
+      <c r="B16" s="8" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>73</v>
+      <c r="B17" s="8" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>74</v>
+      <c r="B18" s="10" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>75</v>
+      <c r="B19" s="11" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>76</v>
+      <c r="B20" s="11" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="12" t="s">
-        <v>77</v>
+      <c r="B21" s="11" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>78</v>
+      <c r="B22" s="11" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="12" t="s">
-        <v>79</v>
+      <c r="B23" s="11" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>80</v>
+      <c r="B24" s="11" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>81</v>
+      <c r="B25" s="11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="13" t="s">
-        <v>82</v>
+      <c r="B26" s="12" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="13" t="s">
-        <v>83</v>
+      <c r="B27" s="12" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>84</v>
+      <c r="B28" s="12" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="13" t="s">
-        <v>85</v>
+      <c r="B29" s="12" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="13" t="s">
-        <v>86</v>
+      <c r="B30" s="12" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="13" t="s">
-        <v>87</v>
+      <c r="B31" s="12" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="15" t="s">
-        <v>88</v>
+      <c r="B32" s="14" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="15" t="s">
-        <v>89</v>
+      <c r="B33" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="15" t="s">
-        <v>90</v>
+      <c r="B34" s="14" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="15" t="s">
-        <v>91</v>
+      <c r="B35" s="14" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="15" t="s">
-        <v>92</v>
+      <c r="B36" s="14" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="15" t="s">
-        <v>93</v>
+      <c r="B37" s="14" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="15" t="s">
-        <v>94</v>
+      <c r="B38" s="14" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1794,7 +1792,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B9">
-    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="blank">
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="blank">
       <formula>NOT(ISERROR(SEARCH("blank",B2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="qq">

</xml_diff>